<commit_message>
adding multiple items  in PO and WO , fix the Unit issue
</commit_message>
<xml_diff>
--- a/modules/purchase/uploads/file_sample/Sample_import_item_en.xlsx
+++ b/modules/purchase/uploads/file_sample/Sample_import_item_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanjay Kothari\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6B1C12-ACF9-43F4-9411-D5B3E7F10C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA61420-E9CF-40FB-8D37-5ACD9109C2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Quantity</t>
   </si>
@@ -33,38 +33,14 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t xml:space="preserve"> Item Description</t>
-  </si>
-  <si>
-    <r>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>)Product Code</t>
-    </r>
+    <t xml:space="preserve"> (*)Item Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,20 +53,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -107,22 +69,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -143,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,13 +103,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -441,27 +389,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="53.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.21875" style="3"/>
+    <col min="1" max="3" width="53.5546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.21875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>